<commit_message>
x not in list corrected
</commit_message>
<xml_diff>
--- a/status/status.xlsx
+++ b/status/status.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,26 +453,65 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>soxy.com.json</t>
+          <t>1999beauty.com.json</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>786cosmetics.com_2.json</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>94</v>
+      </c>
+      <c r="C3" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>beautysociety.com_9.json</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>17</v>
+      </c>
+      <c r="C4" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>soxy.com.json</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>www.als.com_6.json</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B6" t="n">
         <v>877</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C6" t="n">
         <v>656</v>
       </c>
     </row>

</xml_diff>